<commit_message>
Resolução de conflito sobre arquivos de nomes iguais
</commit_message>
<xml_diff>
--- a/musica_500.xlsx
+++ b/musica_500.xlsx
@@ -11,225 +11,170 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Times New Roman"/>
-        <b/>
-        <color rgb="FF000009"/>
-        <sz val="10.0"/>
-      </rPr>
-      <t>ROSA MARIA MACHADO BARBOSA</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Times New Roman"/>
-        <b/>
-        <color rgb="FF000009"/>
-        <sz val="10.0"/>
-      </rPr>
-      <t>VICENTE AUGUSTO CIMINO</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Times New Roman"/>
-        <b/>
-        <color rgb="FF000009"/>
-        <sz val="10.0"/>
-      </rPr>
-      <t>LUCÍLIA CHRISPIM CORRÊA</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Times New Roman"/>
-        <b/>
-        <color rgb="FF000009"/>
-        <sz val="10.0"/>
-      </rPr>
-      <t>MARIA APARECIDA DOS SANTOS FERREIRA</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Times New Roman"/>
-        <b/>
-        <color rgb="FF000009"/>
-        <sz val="10.0"/>
-      </rPr>
-      <t>MARIA LUIZA MAZZOCCOLI ALVIM</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Times New Roman"/>
-        <b/>
-        <color rgb="FF000009"/>
-        <sz val="10.0"/>
-      </rPr>
-      <t>RENATA COIMBRA ALVES</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Times New Roman"/>
-        <b/>
-        <color rgb="FF000009"/>
-        <sz val="10.0"/>
-      </rPr>
-      <t>MARCOS PAULO LIMA LOPES</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Times New Roman"/>
-        <b/>
-        <color rgb="FF000009"/>
-        <sz val="10.0"/>
-      </rPr>
-      <t>FERNANDA APARECIDA DA SILVA</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Times New Roman"/>
-        <b/>
-        <color rgb="FF000009"/>
-        <sz val="10.0"/>
-      </rPr>
-      <t>LEONARDO COELHO DUARTE</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Times New Roman"/>
-        <b/>
-        <color rgb="FF000009"/>
-        <sz val="10.0"/>
-      </rPr>
-      <t>MONIQUE MAGALHÃES LEITÃO</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Times New Roman"/>
-        <b/>
-        <color rgb="FF000009"/>
-        <sz val="10.0"/>
-      </rPr>
-      <t>FABRÍCIA MENEZES DE ALMEIDA SILVA LOPES</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Times New Roman"/>
-        <b/>
-        <color rgb="FF000009"/>
-        <sz val="10.0"/>
-      </rPr>
-      <t>ALINE HENRIQUES DA SILVA</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Times New Roman"/>
-        <b/>
-        <color rgb="FF000009"/>
-        <sz val="10.0"/>
-      </rPr>
-      <t>VANESSA FONSECA PONCIO</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Times New Roman"/>
-        <b/>
-        <color rgb="FF000009"/>
-        <sz val="10.0"/>
-      </rPr>
-      <t>LEANDRO MIRANDA ELIAS</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Times New Roman"/>
-        <b/>
-        <color rgb="FF000009"/>
-        <sz val="10.0"/>
-      </rPr>
-      <t>ALEXANDRE DA SILVA CORTEZ</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Times New Roman"/>
-        <b/>
-        <color rgb="FF000009"/>
-        <sz val="10.0"/>
-      </rPr>
-      <t>MARCUS VINICIUS MENDONÇA BARROSO</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Times New Roman"/>
-        <b/>
-        <color rgb="FF000009"/>
-        <sz val="10.0"/>
-      </rPr>
-      <t>PÂMELA RAFAELA DA COSTA FERNANDES</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Times New Roman"/>
-        <b/>
-        <color rgb="FF000009"/>
-        <sz val="10.0"/>
-      </rPr>
-      <t>ANA CRISTINA DANTAS CORDEIRO DE OLIVEIRA</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Times New Roman"/>
-        <b/>
-        <color rgb="FF000009"/>
-        <sz val="10.0"/>
-      </rPr>
-      <t>ROZIANE DOMINGOS DE OLIVEIRA</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Times New Roman"/>
-        <b/>
-        <color rgb="FF000009"/>
-        <sz val="10.0"/>
-      </rPr>
-      <t>JOSE MARIO DE OLIVEIRA</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Times New Roman"/>
+        <b/>
+        <color rgb="FF000009"/>
+        <sz val="10.0"/>
+      </rPr>
+      <t>DENISE MENDES DE GONCALVES</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Times New Roman"/>
+        <b/>
+        <color rgb="FF000009"/>
+        <sz val="10.0"/>
+      </rPr>
+      <t>GISELLE CAMPOS PEREIRA</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Times New Roman"/>
+        <b/>
+        <color rgb="FF000009"/>
+        <sz val="10.0"/>
+      </rPr>
+      <t>LARA DE PAULA CANDIDO</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Times New Roman"/>
+        <b/>
+        <color rgb="FF000009"/>
+        <sz val="10.0"/>
+      </rPr>
+      <t>SARA CRISTINA DE ALMEIDA</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Times New Roman"/>
+        <b/>
+        <color rgb="FF000009"/>
+        <sz val="10.0"/>
+      </rPr>
+      <t>LUCIANO NAZAR DE OLIVEIRA</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Times New Roman"/>
+        <b/>
+        <color rgb="FF000009"/>
+        <sz val="10.0"/>
+      </rPr>
+      <t>JESILEINE DA SILVA VALÉRIO ANDRÉS</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Times New Roman"/>
+        <b/>
+        <color rgb="FF000009"/>
+        <sz val="10.0"/>
+      </rPr>
+      <t>ALMIR CALEBE MARCIÃO DOS SANTOS</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Times New Roman"/>
+        <b/>
+        <color rgb="FF000009"/>
+        <sz val="10.0"/>
+      </rPr>
+      <t>TÚLIO EDSON BESSA ANDRADE</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Times New Roman"/>
+        <b/>
+        <color rgb="FF000009"/>
+        <sz val="10.0"/>
+      </rPr>
+      <t>HIAGO BORDIM PEREIRA</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Times New Roman"/>
+        <b/>
+        <color rgb="FF000009"/>
+        <sz val="10.0"/>
+      </rPr>
+      <t>MARCUS VINÍCIUS DE OLIVEIRA MACIEL</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Times New Roman"/>
+        <b/>
+        <color rgb="FF000009"/>
+        <sz val="10.0"/>
+      </rPr>
+      <t>GABRIELA AMORIM FERREIRA DA COSTA</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Times New Roman"/>
+        <b/>
+        <color rgb="FF000009"/>
+        <sz val="10.0"/>
+      </rPr>
+      <t>MARCOS BARBOSA BRAGA</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Times New Roman"/>
+        <b/>
+        <color rgb="FF000009"/>
+        <sz val="10.0"/>
+      </rPr>
+      <t>FERNANDO SANTOS DE OLIVEIRA</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Times New Roman"/>
+        <b/>
+        <color rgb="FF000009"/>
+        <sz val="10.0"/>
+      </rPr>
+      <t>LILIAN DE CASSIA PINTO DE OLIVEIRA</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Times New Roman"/>
+        <b/>
+        <color rgb="FF000009"/>
+        <sz val="10.0"/>
+      </rPr>
+      <t>RAQUEL DE SOUZA PEREIRA</t>
     </r>
   </si>
   <si>
@@ -240,6 +185,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="###0;###0"/>
+  </numFmts>
   <fonts count="4">
     <font>
       <sz val="10.0"/>
@@ -258,8 +206,10 @@
       <name val="Times New Roman"/>
     </font>
     <font>
+      <b/>
       <color theme="1"/>
-      <name val="Times New Roman"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -290,21 +240,18 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="1" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf borderId="1" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="top" wrapText="1"/>
+      <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -522,12 +469,12 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="2" max="2" width="34.63"/>
+    <col customWidth="1" min="2" max="2" width="44.75"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1">
-        <v>9.0</v>
+        <v>29.0</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -535,7 +482,7 @@
     </row>
     <row r="2">
       <c r="A2" s="1">
-        <v>10.0</v>
+        <v>30.0</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>1</v>
@@ -543,7 +490,7 @@
     </row>
     <row r="3">
       <c r="A3" s="1">
-        <v>11.0</v>
+        <v>31.0</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>2</v>
@@ -551,7 +498,7 @@
     </row>
     <row r="4">
       <c r="A4" s="1">
-        <v>12.0</v>
+        <v>32.0</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>3</v>
@@ -559,7 +506,7 @@
     </row>
     <row r="5">
       <c r="A5" s="1">
-        <v>13.0</v>
+        <v>33.0</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>4</v>
@@ -567,7 +514,7 @@
     </row>
     <row r="6">
       <c r="A6" s="1">
-        <v>14.0</v>
+        <v>34.0</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>5</v>
@@ -575,7 +522,7 @@
     </row>
     <row r="7">
       <c r="A7" s="1">
-        <v>15.0</v>
+        <v>35.0</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>6</v>
@@ -583,7 +530,7 @@
     </row>
     <row r="8">
       <c r="A8" s="1">
-        <v>16.0</v>
+        <v>36.0</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>7</v>
@@ -591,7 +538,7 @@
     </row>
     <row r="9">
       <c r="A9" s="1">
-        <v>17.0</v>
+        <v>37.0</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>8</v>
@@ -599,7 +546,7 @@
     </row>
     <row r="10">
       <c r="A10" s="1">
-        <v>18.0</v>
+        <v>38.0</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>9</v>
@@ -607,7 +554,7 @@
     </row>
     <row r="11">
       <c r="A11" s="1">
-        <v>19.0</v>
+        <v>39.0</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>10</v>
@@ -615,7 +562,7 @@
     </row>
     <row r="12">
       <c r="A12" s="1">
-        <v>20.0</v>
+        <v>40.0</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>11</v>
@@ -623,7 +570,7 @@
     </row>
     <row r="13">
       <c r="A13" s="1">
-        <v>21.0</v>
+        <v>41.0</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>12</v>
@@ -631,7 +578,7 @@
     </row>
     <row r="14">
       <c r="A14" s="1">
-        <v>22.0</v>
+        <v>42.0</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>13</v>
@@ -639,56 +586,15 @@
     </row>
     <row r="15">
       <c r="A15" s="1">
-        <v>23.0</v>
+        <v>43.0</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="1">
-        <v>24.0</v>
-      </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="3" t="s">
         <v>15</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="1">
-        <v>25.0</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="1">
-        <v>26.0</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="1">
-        <v>27.0</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="1">
-        <v>28.0</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="3"/>
-      <c r="B21" s="4" t="s">
-        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Edição da lista de música
</commit_message>
<xml_diff>
--- a/musica_500.xlsx
+++ b/musica_500.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t xml:space="preserve">RODRIGO CANDIDO PEREIRA DA SILVA</t>
   </si>
@@ -53,9 +53,6 @@
   </si>
   <si>
     <t xml:space="preserve">RAMON UZIEL COSTA DO NASCI- MENTO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Item 4.5 do edital</t>
   </si>
   <si>
     <t xml:space="preserve">JULIANA FELISBINA FERREIRA DOS SANTOS</t>
@@ -198,17 +195,21 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -400,10 +401,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B30"/>
+  <dimension ref="A1:B1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B31" activeCellId="0" sqref="B31"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D13" activeCellId="0" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -498,7 +499,7 @@
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="n">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>11</v>
@@ -506,7 +507,7 @@
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="n">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>12</v>
@@ -514,7 +515,7 @@
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="n">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>13</v>
@@ -522,7 +523,7 @@
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="n">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>14</v>
@@ -530,7 +531,7 @@
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="n">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>15</v>
@@ -538,7 +539,7 @@
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="n">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>16</v>
@@ -546,7 +547,7 @@
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="n">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>17</v>
@@ -554,7 +555,7 @@
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="n">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>18</v>
@@ -562,7 +563,7 @@
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="n">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>19</v>
@@ -570,7 +571,7 @@
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="n">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>20</v>
@@ -578,7 +579,7 @@
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="n">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>21</v>
@@ -586,7 +587,7 @@
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="n">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>22</v>
@@ -594,7 +595,7 @@
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="n">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>23</v>
@@ -602,7 +603,7 @@
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="n">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>24</v>
@@ -610,7 +611,7 @@
     </row>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="n">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>25</v>
@@ -618,7 +619,7 @@
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="n">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>26</v>
@@ -626,25 +627,18 @@
     </row>
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="n">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="1" t="n">
-        <v>80</v>
-      </c>
-      <c r="B29" s="2" t="s">
+    <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B29" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B30" s="0" t="s">
-        <v>29</v>
-      </c>
-    </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>